<commit_message>
ajout d'un fichier xls pour les meta data et integration dans index et fiche_projet.php
</commit_message>
<xml_diff>
--- a/data/data_meta.xlsx
+++ b/data/data_meta.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A6D9AF-A9F5-4671-9D35-5B4F4C11FC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,103 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>canonical url</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Portfolio – Dimitri Lefebvre</t>
+  </si>
+  <si>
+    <t>Portfolio de Dimitri Lefebvre, Data Analyst certifié PL300 en Power BI, expert en data visualisation, computer vision, Python, SQL et HTML/CSS. 17 ans d'expérience dans l'industrie chimique appliquée aux industries de process (chimie, agroalimentaire, pharma).</t>
+  </si>
+  <si>
+    <t>Data Analyst, dataviz, Power BI, PL300, Computer Vision, Python, HTML, CSS, SQL, Industrie Chimique, Agroalimentaire, Pharma</t>
+  </si>
+  <si>
+    <t>https://www.portfolio-dimitri-lefebvre.fr/</t>
+  </si>
+  <si>
+    <t>images/icones/favicon.ico</t>
+  </si>
+  <si>
+    <t>Data Analyst certifié RNCP, certifié PL300, spécialisé en dataviz, computer vision et SQL. Découvrez mes projets et mon parcours professionnel.</t>
+  </si>
+  <si>
+    <t>https://www.portfolio-dimitri-lefebvre.fr/images/og-image.jpg</t>
+  </si>
+  <si>
+    <t>open Graph Réseaux Sociaux og:title</t>
+  </si>
+  <si>
+    <t>open Graph Réseaux Sociaux og:description</t>
+  </si>
+  <si>
+    <t>open Graph Réseaux Sociaux og:image</t>
+  </si>
+  <si>
+    <t>open Graph Réseaux Sociaux og:url</t>
+  </si>
+  <si>
+    <t>applicationldjson</t>
+  </si>
+  <si>
+    <t>{
+        "@context": "https://schema.org",
+        "@type": "Person",
+        "name": "Lefebvre Dimitri",
+        "jobTitle": "Data Analyst",
+        "url": "https://www.portfolio-dimitri-lefebvre.fr",
+        "description": "Data Analyst certifié PL300, spécialisé en dataviz, computer vision, Python, SQL, HTML et CSS avec 17 ans d'expérience dans l'industrie chimique appliquée aux industries de process.",
+        "knowsAbout": [
+            "Data Visualisation",
+            "Power BI",
+            "Computer Vision",
+            "Python",
+            "SQL",
+            "HTML",
+            "CSS",
+            "Industrie Chimique",
+            "Agroalimentaire",
+            "Pharma",
+            "Industrie de process"
+        ],
+        "certifications": "PL300",
+        "sameAs": [
+            "https://www.linkedin.com/in/dim-lefebvre60"
+        ]
+    }</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +143,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +441,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="162" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{E6BCFAE4-67A5-4964-8449-A8BB1DC94C7B}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{A821EB2B-8D99-429D-B5A3-6AC6C7827F12}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout des fichiers exemple en modifiant le gitignore
</commit_message>
<xml_diff>
--- a/data/data_meta.xlsx
+++ b/data/data_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A6D9AF-A9F5-4671-9D35-5B4F4C11FC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B89166-A184-4E1A-8E83-77A82315990A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,13 +54,7 @@
     <t>https://www.portfolio-dimitri-lefebvre.fr/</t>
   </si>
   <si>
-    <t>images/icones/favicon.ico</t>
-  </si>
-  <si>
     <t>Data Analyst certifié RNCP, certifié PL300, spécialisé en dataviz, computer vision et SQL. Découvrez mes projets et mon parcours professionnel.</t>
-  </si>
-  <si>
-    <t>https://www.portfolio-dimitri-lefebvre.fr/images/og-image.jpg</t>
   </si>
   <si>
     <t>open Graph Réseaux Sociaux og:title</t>
@@ -103,6 +97,12 @@
             "https://www.linkedin.com/in/dim-lefebvre60"
         ]
     }</t>
+  </si>
+  <si>
+    <t>https://www.portfolio-dimitri-lefebvre.fr/www/images/portraits/DL_gris.png</t>
+  </si>
+  <si>
+    <t>images/icons/favicon.ico</t>
   </si>
 </sst>
 </file>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,12 +491,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -504,23 +504,23 @@
     </row>
     <row r="7" spans="1:2" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -528,10 +528,10 @@
     </row>
     <row r="10" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>